<commit_message>
refactor: Elimina los campos del xlsx del participante
</commit_message>
<xml_diff>
--- a/src/assets/archives/participantes.xlsx
+++ b/src/assets/archives/participantes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utaedu-my.sharepoint.com/personal/kcayo6155_uta_edu_ec/Documents/Imágenes/DAS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aplicaciones_web_movil\Certyget\src\assets\archives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{048A8364-5760-4B03-B714-DCA66F6D8C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFFC71A9-59CC-4CDA-9382-014D25FE1759}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CA5180-B772-46F3-B678-1F6985DC1292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,21 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{28D75815-8B4A-48AF-83E0-6543D614C4E5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Teléfono</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{1C11B85B-B7F5-41DF-B522-0B91DB2093AA}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{1C11B85B-B7F5-41DF-B522-0B91DB2093AA}">
       <text>
         <r>
           <rPr>
@@ -123,80 +109,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{A9007432-BA76-42A8-B615-04888375DB34}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Dirección</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{CE985FEC-535C-4051-98C3-763638AE3A6B}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ciudad</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{710CC572-EFE1-4482-98C1-B75861C0A6A2}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Carrera de estudio</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{483A8E31-FDA6-4CB0-8D14-5210197FA53C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Facultad de estudio</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{DBA77864-D664-4DEA-9AAE-F602E5EC6C77}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Universidad</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ced_par</t>
   </si>
@@ -213,32 +131,14 @@
     <t>ape_mat_par</t>
   </si>
   <si>
-    <t>telf_par</t>
-  </si>
-  <si>
     <t>email_par</t>
-  </si>
-  <si>
-    <t>dir_par</t>
-  </si>
-  <si>
-    <t>ciud_par</t>
-  </si>
-  <si>
-    <t>carrera_par</t>
-  </si>
-  <si>
-    <t>fac_par</t>
-  </si>
-  <si>
-    <t>uni_par</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,12 +272,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1085,15 +979,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1112,24 +1014,6 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>